<commit_message>
DVK Volitve EP2024 update 🤖
</commit_message>
<xml_diff>
--- a/data/ep2024/izvoz.xlsx
+++ b/data/ep2024/izvoz.xlsx
@@ -25,7 +25,7 @@
     <t>Podatki osveženi:</t>
   </si>
   <si>
-    <t>21:10</t>
+    <t>21:15</t>
   </si>
   <si>
     <t>Volilna enota</t>
@@ -10184,7 +10184,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="4">
-        <v>45452.881944444445</v>
+        <v>45452.885416666664</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>3</v>
@@ -10287,13 +10287,13 @@
     </row>
     <row r="6">
       <c r="C6" s="0">
-        <v>1689499</v>
+        <v>1689501</v>
       </c>
       <c r="D6" s="0">
-        <v>444857</v>
+        <v>446149</v>
       </c>
       <c r="E6" s="8">
-        <v>0.2633</v>
+        <v>0.2641</v>
       </c>
     </row>
     <row r="7">
@@ -10304,10 +10304,10 @@
         <v>208088</v>
       </c>
       <c r="D7" s="0">
-        <v>58251</v>
+        <v>58398</v>
       </c>
       <c r="E7" s="8">
-        <v>0.2799</v>
+        <v>0.2806</v>
       </c>
     </row>
     <row r="8">
@@ -10321,10 +10321,10 @@
         <v>25954</v>
       </c>
       <c r="D8" s="0">
-        <v>6003</v>
+        <v>6037</v>
       </c>
       <c r="E8" s="8">
-        <v>0.2313</v>
+        <v>0.2326</v>
       </c>
     </row>
     <row r="9">
@@ -10338,10 +10338,10 @@
         <v>13412</v>
       </c>
       <c r="D9" s="0">
-        <v>4035</v>
+        <v>4076</v>
       </c>
       <c r="E9" s="8">
-        <v>0.3008</v>
+        <v>0.3039</v>
       </c>
     </row>
     <row r="10">
@@ -10355,10 +10355,10 @@
         <v>15875</v>
       </c>
       <c r="D10" s="0">
-        <v>4505</v>
+        <v>4527</v>
       </c>
       <c r="E10" s="8">
-        <v>0.2838</v>
+        <v>0.2852</v>
       </c>
     </row>
     <row r="11">
@@ -10406,10 +10406,10 @@
         <v>24387</v>
       </c>
       <c r="D13" s="0">
-        <v>8374</v>
+        <v>8401</v>
       </c>
       <c r="E13" s="8">
-        <v>0.3434</v>
+        <v>0.3445</v>
       </c>
     </row>
     <row r="14">
@@ -10457,10 +10457,10 @@
         <v>15430</v>
       </c>
       <c r="D16" s="0">
-        <v>5371</v>
+        <v>5394</v>
       </c>
       <c r="E16" s="8">
-        <v>0.3481</v>
+        <v>0.3496</v>
       </c>
     </row>
     <row r="17">
@@ -10505,10 +10505,10 @@
         <v>208558</v>
       </c>
       <c r="D19" s="0">
-        <v>53055</v>
+        <v>53148</v>
       </c>
       <c r="E19" s="8">
-        <v>0.2544</v>
+        <v>0.2548</v>
       </c>
     </row>
     <row r="20">
@@ -10522,10 +10522,10 @@
         <v>15809</v>
       </c>
       <c r="D20" s="0">
-        <v>5342</v>
+        <v>5353</v>
       </c>
       <c r="E20" s="8">
-        <v>0.3379</v>
+        <v>0.3386</v>
       </c>
     </row>
     <row r="21">
@@ -10556,10 +10556,10 @@
         <v>12475</v>
       </c>
       <c r="D22" s="0">
-        <v>2543</v>
+        <v>2560</v>
       </c>
       <c r="E22" s="8">
-        <v>0.2038</v>
+        <v>0.2052</v>
       </c>
     </row>
     <row r="23">
@@ -10573,10 +10573,10 @@
         <v>18284</v>
       </c>
       <c r="D23" s="0">
-        <v>3676</v>
+        <v>3712</v>
       </c>
       <c r="E23" s="8">
-        <v>0.2011</v>
+        <v>0.203</v>
       </c>
     </row>
     <row r="24">
@@ -10590,10 +10590,10 @@
         <v>25254</v>
       </c>
       <c r="D24" s="0">
-        <v>5680</v>
+        <v>5690</v>
       </c>
       <c r="E24" s="8">
-        <v>0.2249</v>
+        <v>0.2253</v>
       </c>
     </row>
     <row r="25">
@@ -10624,10 +10624,10 @@
         <v>12655</v>
       </c>
       <c r="D26" s="0">
-        <v>2729</v>
+        <v>2737</v>
       </c>
       <c r="E26" s="8">
-        <v>0.2156</v>
+        <v>0.2163</v>
       </c>
     </row>
     <row r="27">
@@ -10641,10 +10641,10 @@
         <v>18040</v>
       </c>
       <c r="D27" s="0">
-        <v>4716</v>
+        <v>4727</v>
       </c>
       <c r="E27" s="8">
-        <v>0.2614</v>
+        <v>0.262</v>
       </c>
     </row>
     <row r="28">
@@ -10706,10 +10706,10 @@
         <v>219992</v>
       </c>
       <c r="D31" s="0">
-        <v>62524</v>
+        <v>62597</v>
       </c>
       <c r="E31" s="8">
-        <v>0.2842</v>
+        <v>0.2845</v>
       </c>
     </row>
     <row r="32">
@@ -10740,10 +10740,10 @@
         <v>20176</v>
       </c>
       <c r="D33" s="0">
-        <v>5742</v>
+        <v>5790</v>
       </c>
       <c r="E33" s="8">
-        <v>0.2846</v>
+        <v>0.287</v>
       </c>
     </row>
     <row r="34">
@@ -10808,10 +10808,10 @@
         <v>21969</v>
       </c>
       <c r="D37" s="0">
-        <v>6023</v>
+        <v>6048</v>
       </c>
       <c r="E37" s="8">
-        <v>0.2742</v>
+        <v>0.2753</v>
       </c>
     </row>
     <row r="38">
@@ -10907,10 +10907,10 @@
         <v>208624</v>
       </c>
       <c r="D43" s="0">
-        <v>54097</v>
+        <v>54141</v>
       </c>
       <c r="E43" s="8">
-        <v>0.2593</v>
+        <v>0.2595</v>
       </c>
     </row>
     <row r="44">
@@ -11077,10 +11077,10 @@
         <v>24733</v>
       </c>
       <c r="D53" s="0">
-        <v>6143</v>
+        <v>6187</v>
       </c>
       <c r="E53" s="8">
-        <v>0.2484</v>
+        <v>0.2502</v>
       </c>
     </row>
     <row r="54">
@@ -11108,10 +11108,10 @@
         <v>210445</v>
       </c>
       <c r="D55" s="0">
-        <v>55175</v>
+        <v>55395</v>
       </c>
       <c r="E55" s="8">
-        <v>0.2622</v>
+        <v>0.2632</v>
       </c>
     </row>
     <row r="56">
@@ -11125,10 +11125,10 @@
         <v>17035</v>
       </c>
       <c r="D56" s="0">
-        <v>4506</v>
+        <v>4521</v>
       </c>
       <c r="E56" s="8">
-        <v>0.2645</v>
+        <v>0.2654</v>
       </c>
     </row>
     <row r="57">
@@ -11142,10 +11142,10 @@
         <v>29350</v>
       </c>
       <c r="D57" s="0">
-        <v>8359</v>
+        <v>8372</v>
       </c>
       <c r="E57" s="8">
-        <v>0.2848</v>
+        <v>0.2852</v>
       </c>
     </row>
     <row r="58">
@@ -11176,10 +11176,10 @@
         <v>18123</v>
       </c>
       <c r="D59" s="0">
-        <v>4739</v>
+        <v>4767</v>
       </c>
       <c r="E59" s="8">
-        <v>0.2615</v>
+        <v>0.263</v>
       </c>
     </row>
     <row r="60">
@@ -11193,10 +11193,10 @@
         <v>18748</v>
       </c>
       <c r="D60" s="0">
-        <v>5555</v>
+        <v>5583</v>
       </c>
       <c r="E60" s="8">
-        <v>0.2963</v>
+        <v>0.2978</v>
       </c>
     </row>
     <row r="61">
@@ -11244,10 +11244,10 @@
         <v>17242</v>
       </c>
       <c r="D63" s="0">
-        <v>4456</v>
+        <v>4562</v>
       </c>
       <c r="E63" s="8">
-        <v>0.2584</v>
+        <v>0.2646</v>
       </c>
     </row>
     <row r="64">
@@ -11295,10 +11295,10 @@
         <v>20409</v>
       </c>
       <c r="D66" s="0">
-        <v>5113</v>
+        <v>5143</v>
       </c>
       <c r="E66" s="8">
-        <v>0.2505</v>
+        <v>0.252</v>
       </c>
     </row>
     <row r="67">
@@ -11309,10 +11309,10 @@
         <v>217449</v>
       </c>
       <c r="D67" s="0">
-        <v>56847</v>
+        <v>57001</v>
       </c>
       <c r="E67" s="8">
-        <v>0.2614</v>
+        <v>0.2621</v>
       </c>
     </row>
     <row r="68">
@@ -11326,10 +11326,10 @@
         <v>22687</v>
       </c>
       <c r="D68" s="0">
-        <v>5809</v>
+        <v>5835</v>
       </c>
       <c r="E68" s="8">
-        <v>0.256</v>
+        <v>0.2572</v>
       </c>
     </row>
     <row r="69">
@@ -11343,10 +11343,10 @@
         <v>24393</v>
       </c>
       <c r="D69" s="0">
-        <v>6412</v>
+        <v>6455</v>
       </c>
       <c r="E69" s="8">
-        <v>0.2629</v>
+        <v>0.2646</v>
       </c>
     </row>
     <row r="70">
@@ -11394,10 +11394,10 @@
         <v>21167</v>
       </c>
       <c r="D72" s="0">
-        <v>4805</v>
+        <v>4819</v>
       </c>
       <c r="E72" s="8">
-        <v>0.227</v>
+        <v>0.2277</v>
       </c>
     </row>
     <row r="73">
@@ -11411,10 +11411,10 @@
         <v>23168</v>
       </c>
       <c r="D73" s="0">
-        <v>6372</v>
+        <v>6391</v>
       </c>
       <c r="E73" s="8">
-        <v>0.275</v>
+        <v>0.2759</v>
       </c>
     </row>
     <row r="74">
@@ -11428,10 +11428,10 @@
         <v>17021</v>
       </c>
       <c r="D74" s="0">
-        <v>4614</v>
+        <v>4628</v>
       </c>
       <c r="E74" s="8">
-        <v>0.2711</v>
+        <v>0.2719</v>
       </c>
     </row>
     <row r="75">
@@ -11462,10 +11462,10 @@
         <v>17172</v>
       </c>
       <c r="D76" s="0">
-        <v>4962</v>
+        <v>5000</v>
       </c>
       <c r="E76" s="8">
-        <v>0.289</v>
+        <v>0.2912</v>
       </c>
     </row>
     <row r="77">
@@ -11510,10 +11510,10 @@
         <v>206664</v>
       </c>
       <c r="D79" s="0">
-        <v>47852</v>
+        <v>48053</v>
       </c>
       <c r="E79" s="8">
-        <v>0.2315</v>
+        <v>0.2325</v>
       </c>
     </row>
     <row r="80">
@@ -11527,10 +11527,10 @@
         <v>27753</v>
       </c>
       <c r="D80" s="0">
-        <v>4837</v>
+        <v>4845</v>
       </c>
       <c r="E80" s="8">
-        <v>0.1743</v>
+        <v>0.1746</v>
       </c>
     </row>
     <row r="81">
@@ -11544,10 +11544,10 @@
         <v>25212</v>
       </c>
       <c r="D81" s="0">
-        <v>6627</v>
+        <v>6651</v>
       </c>
       <c r="E81" s="8">
-        <v>0.2629</v>
+        <v>0.2638</v>
       </c>
     </row>
     <row r="82">
@@ -11612,10 +11612,10 @@
         <v>21076</v>
       </c>
       <c r="D85" s="0">
-        <v>4754</v>
+        <v>4866</v>
       </c>
       <c r="E85" s="8">
-        <v>0.2256</v>
+        <v>0.2309</v>
       </c>
     </row>
     <row r="86">
@@ -11629,10 +11629,10 @@
         <v>17307</v>
       </c>
       <c r="D86" s="0">
-        <v>4122</v>
+        <v>4179</v>
       </c>
       <c r="E86" s="8">
-        <v>0.2382</v>
+        <v>0.2415</v>
       </c>
     </row>
     <row r="87">
@@ -11708,13 +11708,13 @@
         <v>119</v>
       </c>
       <c r="C91" s="0">
-        <v>209675</v>
+        <v>209677</v>
       </c>
       <c r="D91" s="0">
-        <v>53340</v>
+        <v>53665</v>
       </c>
       <c r="E91" s="8">
-        <v>0.2544</v>
+        <v>0.2559</v>
       </c>
     </row>
     <row r="92">
@@ -11728,10 +11728,10 @@
         <v>21145</v>
       </c>
       <c r="D92" s="0">
-        <v>4639</v>
+        <v>4677</v>
       </c>
       <c r="E92" s="8">
-        <v>0.2194</v>
+        <v>0.2212</v>
       </c>
     </row>
     <row r="93">
@@ -11745,10 +11745,10 @@
         <v>14121</v>
       </c>
       <c r="D93" s="0">
-        <v>4041</v>
+        <v>4060</v>
       </c>
       <c r="E93" s="8">
-        <v>0.2862</v>
+        <v>0.2875</v>
       </c>
     </row>
     <row r="94">
@@ -11779,10 +11779,10 @@
         <v>24318</v>
       </c>
       <c r="D95" s="0">
-        <v>6463</v>
+        <v>6498</v>
       </c>
       <c r="E95" s="8">
-        <v>0.2658</v>
+        <v>0.2672</v>
       </c>
     </row>
     <row r="96">
@@ -11796,10 +11796,10 @@
         <v>24845</v>
       </c>
       <c r="D96" s="0">
-        <v>6181</v>
+        <v>6223</v>
       </c>
       <c r="E96" s="8">
-        <v>0.2488</v>
+        <v>0.2505</v>
       </c>
     </row>
     <row r="97">
@@ -11810,13 +11810,13 @@
         <v>125</v>
       </c>
       <c r="C97" s="0">
-        <v>17766</v>
+        <v>17768</v>
       </c>
       <c r="D97" s="0">
-        <v>4712</v>
+        <v>4731</v>
       </c>
       <c r="E97" s="8">
-        <v>0.2652</v>
+        <v>0.2663</v>
       </c>
     </row>
     <row r="98">
@@ -11830,10 +11830,10 @@
         <v>16488</v>
       </c>
       <c r="D98" s="0">
-        <v>4219</v>
+        <v>4244</v>
       </c>
       <c r="E98" s="8">
-        <v>0.2559</v>
+        <v>0.2574</v>
       </c>
     </row>
     <row r="99">
@@ -11847,10 +11847,10 @@
         <v>18016</v>
       </c>
       <c r="D99" s="0">
-        <v>4209</v>
+        <v>4246</v>
       </c>
       <c r="E99" s="8">
-        <v>0.2336</v>
+        <v>0.2357</v>
       </c>
     </row>
     <row r="100">
@@ -11864,10 +11864,10 @@
         <v>21295</v>
       </c>
       <c r="D100" s="0">
-        <v>5980</v>
+        <v>6006</v>
       </c>
       <c r="E100" s="8">
-        <v>0.2808</v>
+        <v>0.282</v>
       </c>
     </row>
     <row r="101">
@@ -11881,10 +11881,10 @@
         <v>17016</v>
       </c>
       <c r="D101" s="0">
-        <v>4507</v>
+        <v>4565</v>
       </c>
       <c r="E101" s="8">
-        <v>0.2649</v>
+        <v>0.2683</v>
       </c>
     </row>
     <row r="102">
@@ -11898,10 +11898,10 @@
         <v>19556</v>
       </c>
       <c r="D102" s="0">
-        <v>4807</v>
+        <v>4833</v>
       </c>
       <c r="E102" s="8">
-        <v>0.2458</v>
+        <v>0.2471</v>
       </c>
     </row>
   </sheetData>
@@ -13956,10 +13956,10 @@
         <v>334</v>
       </c>
       <c r="F16" s="0">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="G16" s="8">
-        <v>0.3683</v>
+        <v>0.4701</v>
       </c>
     </row>
     <row r="17">
@@ -14922,10 +14922,10 @@
         <v>243</v>
       </c>
       <c r="F58" s="0">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="G58" s="8">
-        <v>0.3374</v>
+        <v>0.5062</v>
       </c>
     </row>
     <row r="59">
@@ -15497,10 +15497,10 @@
         <v>145</v>
       </c>
       <c r="F83" s="0">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="G83" s="8">
-        <v>0.3103</v>
+        <v>0.4621</v>
       </c>
     </row>
     <row r="84">
@@ -17843,10 +17843,10 @@
         <v>300</v>
       </c>
       <c r="F185" s="0">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="G185" s="8">
-        <v>0.4167</v>
+        <v>0.5067</v>
       </c>
     </row>
     <row r="186">
@@ -19223,7 +19223,7 @@
         <v>0</v>
       </c>
       <c r="F245" s="0">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="G245" s="8">
         <v>0</v>
@@ -19821,10 +19821,10 @@
         <v>282</v>
       </c>
       <c r="F271" s="0">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="G271" s="8">
-        <v>0.461</v>
+        <v>0.5426</v>
       </c>
     </row>
     <row r="272">
@@ -23202,10 +23202,10 @@
         <v>83</v>
       </c>
       <c r="F418" s="0">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="G418" s="8">
-        <v>0.506</v>
+        <v>0.6386</v>
       </c>
     </row>
     <row r="419">
@@ -24490,10 +24490,10 @@
         <v>131</v>
       </c>
       <c r="F474" s="0">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="G474" s="8">
-        <v>0.3511</v>
+        <v>0.4809</v>
       </c>
     </row>
     <row r="475">
@@ -25042,10 +25042,10 @@
         <v>520</v>
       </c>
       <c r="F498" s="0">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="G498" s="8">
-        <v>0.1885</v>
+        <v>0.2577</v>
       </c>
     </row>
     <row r="499">
@@ -25985,10 +25985,10 @@
         <v>42</v>
       </c>
       <c r="F539" s="0">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G539" s="8">
-        <v>0.2619</v>
+        <v>0.4286</v>
       </c>
     </row>
     <row r="540">
@@ -26146,10 +26146,10 @@
         <v>42</v>
       </c>
       <c r="F546" s="0">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G546" s="8">
-        <v>0.2143</v>
+        <v>0.2857</v>
       </c>
     </row>
     <row r="547">
@@ -29435,10 +29435,10 @@
         <v>96</v>
       </c>
       <c r="F689" s="0">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G689" s="8">
-        <v>0.3438</v>
+        <v>0.4271</v>
       </c>
     </row>
     <row r="690">
@@ -29941,10 +29941,10 @@
         <v>50</v>
       </c>
       <c r="F711" s="0">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G711" s="8">
-        <v>0.4</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="712">
@@ -35806,10 +35806,10 @@
         <v>428</v>
       </c>
       <c r="F966" s="0">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="G966" s="8">
-        <v>0.25</v>
+        <v>0.3621</v>
       </c>
     </row>
     <row r="967">
@@ -38382,10 +38382,10 @@
         <v>292</v>
       </c>
       <c r="F1078" s="0">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="G1078" s="8">
-        <v>0.4247</v>
+        <v>0.5103</v>
       </c>
     </row>
     <row r="1079">
@@ -44615,7 +44615,7 @@
         <v>0</v>
       </c>
       <c r="F1349" s="0">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="G1349" s="8">
         <v>0</v>
@@ -49123,10 +49123,10 @@
         <v>335</v>
       </c>
       <c r="F1545" s="0">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="G1545" s="8">
-        <v>0.2119</v>
+        <v>0.3433</v>
       </c>
     </row>
     <row r="1546">
@@ -50549,10 +50549,10 @@
         <v>185</v>
       </c>
       <c r="F1607" s="0">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="G1607" s="8">
-        <v>0.1622</v>
+        <v>0.2432</v>
       </c>
     </row>
     <row r="1608">
@@ -51446,10 +51446,10 @@
         <v>251</v>
       </c>
       <c r="F1646" s="0">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="G1646" s="8">
-        <v>0.251</v>
+        <v>0.3028</v>
       </c>
     </row>
     <row r="1647">
@@ -52757,10 +52757,10 @@
         <v>212</v>
       </c>
       <c r="F1703" s="0">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="G1703" s="8">
-        <v>0.3255</v>
+        <v>0.4575</v>
       </c>
     </row>
     <row r="1704">
@@ -53516,10 +53516,10 @@
         <v>241</v>
       </c>
       <c r="F1736" s="0">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="G1736" s="8">
-        <v>0.2697</v>
+        <v>0.3859</v>
       </c>
     </row>
     <row r="1737">
@@ -55264,10 +55264,10 @@
         <v>573</v>
       </c>
       <c r="F1812" s="0">
-        <v>152</v>
+        <v>258</v>
       </c>
       <c r="G1812" s="8">
-        <v>0.2653</v>
+        <v>0.4503</v>
       </c>
     </row>
     <row r="1813">
@@ -57909,10 +57909,10 @@
         <v>233</v>
       </c>
       <c r="F1927" s="0">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="G1927" s="8">
-        <v>0.2017</v>
+        <v>0.3305</v>
       </c>
     </row>
     <row r="1928">
@@ -59289,10 +59289,10 @@
         <v>149</v>
       </c>
       <c r="F1987" s="0">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="G1987" s="8">
-        <v>0.2953</v>
+        <v>0.4698</v>
       </c>
     </row>
     <row r="1988">
@@ -60163,10 +60163,10 @@
         <v>490</v>
       </c>
       <c r="F2025" s="0">
-        <v>111</v>
+        <v>154</v>
       </c>
       <c r="G2025" s="8">
-        <v>0.2265</v>
+        <v>0.3143</v>
       </c>
     </row>
     <row r="2026">
@@ -63682,10 +63682,10 @@
         <v>230</v>
       </c>
       <c r="F2178" s="0">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="G2178" s="8">
-        <v>0.1826</v>
+        <v>0.2435</v>
       </c>
     </row>
     <row r="2179">
@@ -65361,10 +65361,10 @@
         <v>164</v>
       </c>
       <c r="F2251" s="0">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="G2251" s="8">
-        <v>0.2988</v>
+        <v>0.4146</v>
       </c>
     </row>
     <row r="2252">
@@ -66603,10 +66603,10 @@
         <v>93</v>
       </c>
       <c r="F2305" s="0">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="G2305" s="8">
-        <v>0.2581</v>
+        <v>0.4086</v>
       </c>
     </row>
     <row r="2306">
@@ -68282,10 +68282,10 @@
         <v>135</v>
       </c>
       <c r="F2378" s="0">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="G2378" s="8">
-        <v>0.3333</v>
+        <v>0.4889</v>
       </c>
     </row>
     <row r="2379">
@@ -68604,10 +68604,10 @@
         <v>95</v>
       </c>
       <c r="F2392" s="0">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="G2392" s="8">
-        <v>0.2842</v>
+        <v>0.4632</v>
       </c>
     </row>
     <row r="2393">
@@ -71663,10 +71663,10 @@
         <v>82</v>
       </c>
       <c r="F2525" s="0">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="G2525" s="8">
-        <v>0.3293</v>
+        <v>0.4268</v>
       </c>
     </row>
     <row r="2526">
@@ -72514,10 +72514,10 @@
         <v>212</v>
       </c>
       <c r="F2562" s="0">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G2562" s="8">
-        <v>0.2123</v>
+        <v>0.2736</v>
       </c>
     </row>
     <row r="2563">
@@ -72905,10 +72905,10 @@
         <v>169</v>
       </c>
       <c r="F2579" s="0">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="G2579" s="8">
-        <v>0.2071</v>
+        <v>0.2722</v>
       </c>
     </row>
     <row r="2580">
@@ -76470,7 +76470,7 @@
         <v>0</v>
       </c>
       <c r="F2734" s="0">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="G2734" s="8">
         <v>0</v>
@@ -76815,10 +76815,10 @@
         <v>557</v>
       </c>
       <c r="F2749" s="0">
-        <v>127</v>
+        <v>184</v>
       </c>
       <c r="G2749" s="8">
-        <v>0.228</v>
+        <v>0.3303</v>
       </c>
     </row>
     <row r="2750">
@@ -78954,10 +78954,10 @@
         <v>276</v>
       </c>
       <c r="F2842" s="0">
-        <v>77</v>
+        <v>115</v>
       </c>
       <c r="G2842" s="8">
-        <v>0.279</v>
+        <v>0.4167</v>
       </c>
     </row>
     <row r="2843">
@@ -80495,10 +80495,10 @@
         <v>163</v>
       </c>
       <c r="F2909" s="0">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="G2909" s="8">
-        <v>0.3865</v>
+        <v>0.5031</v>
       </c>
     </row>
     <row r="2910">
@@ -82335,10 +82335,10 @@
         <v>192</v>
       </c>
       <c r="F2989" s="0">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="G2989" s="8">
-        <v>0.25</v>
+        <v>0.3906</v>
       </c>
     </row>
     <row r="2990">
@@ -82887,10 +82887,10 @@
         <v>78</v>
       </c>
       <c r="F3013" s="0">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G3013" s="8">
-        <v>0.2821</v>
+        <v>0.3846</v>
       </c>
     </row>
     <row r="3014">
@@ -85003,10 +85003,10 @@
         <v>401</v>
       </c>
       <c r="F3105" s="0">
-        <v>132</v>
+        <v>174</v>
       </c>
       <c r="G3105" s="8">
-        <v>0.3292</v>
+        <v>0.4339</v>
       </c>
     </row>
     <row r="3106">
@@ -85943,13 +85943,13 @@
         <v>3065</v>
       </c>
       <c r="E3146" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F3146" s="0">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="G3146" s="8">
-        <v>0.2334</v>
+        <v>0.2915</v>
       </c>
     </row>
     <row r="3147">
@@ -86912,10 +86912,10 @@
         <v>619</v>
       </c>
       <c r="F3188" s="0">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="G3188" s="8">
-        <v>0.294</v>
+        <v>0.3344</v>
       </c>
     </row>
     <row r="3189">
@@ -87786,10 +87786,10 @@
         <v>294</v>
       </c>
       <c r="F3226" s="0">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="G3226" s="8">
-        <v>0.2109</v>
+        <v>0.3367</v>
       </c>
     </row>
     <row r="3227">
@@ -89189,10 +89189,10 @@
         <v>247</v>
       </c>
       <c r="F3287" s="0">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="G3287" s="8">
-        <v>0.2753</v>
+        <v>0.3806</v>
       </c>
     </row>
     <row r="3288">
@@ -89810,10 +89810,10 @@
         <v>509</v>
       </c>
       <c r="F3314" s="0">
-        <v>141</v>
+        <v>199</v>
       </c>
       <c r="G3314" s="8">
-        <v>0.277</v>
+        <v>0.391</v>
       </c>
     </row>
     <row r="3315">
@@ -90661,10 +90661,10 @@
         <v>80</v>
       </c>
       <c r="F3351" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G3351" s="8">
-        <v>0.1875</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="3352">
@@ -91420,10 +91420,10 @@
         <v>120</v>
       </c>
       <c r="F3384" s="0">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G3384" s="8">
-        <v>0.3083</v>
+        <v>0.4417</v>
       </c>
     </row>
     <row r="3385">

</xml_diff>